<commit_message>
Finish edit photon. Update quotes
</commit_message>
<xml_diff>
--- a/photon/JERcalc.xlsx
+++ b/photon/JERcalc.xlsx
@@ -387,45 +387,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3.7504499999999998</v>
       </c>
@@ -439,7 +439,7 @@
         <v>2.77935</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>5.28128E-2</v>
       </c>
@@ -453,7 +453,37 @@
         <v>4.6705900000000002E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>3.49641</v>
+      </c>
+      <c r="M14">
+        <v>2.7242600000000001</v>
+      </c>
+      <c r="N14">
+        <v>2.6166700000000001</v>
+      </c>
+      <c r="O14">
+        <v>2.7686000000000002</v>
+      </c>
+      <c r="Q14">
+        <f>SQRT(L15^2-L14^2)</f>
+        <v>0.71575629812108477</v>
+      </c>
+      <c r="R14">
+        <f t="shared" ref="R14:T14" si="0">SQRT(M15^2-M14^2)</f>
+        <v>0.85383415093330606</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="0"/>
+        <v>1.267996670027173</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="0"/>
+        <v>1.3704954642756031</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3.8144200000000001</v>
       </c>
@@ -471,19 +501,47 @@
         <v>0.6956469894278291</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="H15:J15" si="0">SQRT(B15^2-B12^2)</f>
+        <f t="shared" ref="H15:J15" si="1">SQRT(B15^2-B12^2)</f>
         <v>0.80556769355529489</v>
       </c>
       <c r="I15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.1830417162551792</v>
       </c>
       <c r="J15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3453510482769913</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <v>3.5689199999999999</v>
+      </c>
+      <c r="M15">
+        <v>2.85493</v>
+      </c>
+      <c r="N15">
+        <v>2.9077099999999998</v>
+      </c>
+      <c r="O15">
+        <v>3.0892400000000002</v>
+      </c>
+      <c r="Q15">
+        <f>SQRT(L16^2-L14^2)</f>
+        <v>1.3926056310025459</v>
+      </c>
+      <c r="R15">
+        <f t="shared" ref="R15:T15" si="2">SQRT(M16^2-M14^2)</f>
+        <v>0.94771874118854438</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="2"/>
+        <v>0.92282704121628367</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="2"/>
+        <v>0.85305029253848763</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>5.2008899999999997E-2</v>
       </c>
@@ -501,19 +559,61 @@
         <v>7.4122314609367135E-2</v>
       </c>
       <c r="H16">
-        <f t="shared" ref="H16:J16" si="1">SQRT((B16)^2+(B13)^2)</f>
+        <f t="shared" ref="H16:J16" si="3">SQRT((B16)^2+(B13)^2)</f>
         <v>6.2973907747415528E-2</v>
       </c>
       <c r="I16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.6903192010466341E-2</v>
       </c>
       <c r="J16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.0310256621420458E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <v>3.7635399999999999</v>
+      </c>
+      <c r="M16">
+        <v>2.8843999999999999</v>
+      </c>
+      <c r="N16">
+        <v>2.7746300000000002</v>
+      </c>
+      <c r="O16">
+        <v>2.8970400000000001</v>
+      </c>
+      <c r="Q16">
+        <f>SQRT(L17^2-L14^2)</f>
+        <v>1.4050165601871034</v>
+      </c>
+      <c r="R16">
+        <f t="shared" ref="R16:T16" si="4">SQRT(M17^2-M14^2)</f>
+        <v>1.0018904505483615</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="4"/>
+        <v>1.1685722800066749</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="4"/>
+        <v>0.93415514905180397</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <v>3.7681499999999999</v>
+      </c>
+      <c r="M17">
+        <v>2.90265</v>
+      </c>
+      <c r="N17">
+        <v>2.8657499999999998</v>
+      </c>
+      <c r="O17">
+        <v>2.9219499999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3.7635399999999999</v>
       </c>
@@ -531,19 +631,19 @@
         <v>0.31362099594893084</v>
       </c>
       <c r="H18">
-        <f t="shared" ref="H18:J18" si="2">SQRT(B18^2-B12^2)</f>
+        <f t="shared" ref="H18:J18" si="5">SQRT(B18^2-B12^2)</f>
         <v>0.35427899514365568</v>
       </c>
       <c r="I18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>#NUM!</v>
       </c>
       <c r="J18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.81734591153317715</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4.8263800000000003E-2</v>
       </c>
@@ -561,39 +661,39 @@
         <v>7.1544295609643122E-2</v>
       </c>
       <c r="H19">
-        <f t="shared" ref="H19:J19" si="3">SQRT((B19)^2+(B13)^2)</f>
+        <f t="shared" ref="H19:J19" si="6">SQRT((B19)^2+(B13)^2)</f>
         <v>6.0172084259895807E-2</v>
       </c>
       <c r="I19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.3623626924146045E-2</v>
       </c>
       <c r="J19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5.9393578733815997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>10</v>
       </c>

</xml_diff>